<commit_message>
formate cc5 is added
</commit_message>
<xml_diff>
--- a/templates/excel/format CC5.xlsx
+++ b/templates/excel/format CC5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github-desktop\UI\QA\CA-Dev-New\backend\templates\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github-desktop\UI\DEV\CA-DEV\CA-BACKEND-DEV\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA3A548-59B5-4F0F-A4D9-E18E0C060BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3055EF-ACAC-41D7-9C5D-048527111C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3088,6 +3088,108 @@
     <xf numFmtId="1" fontId="10" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3097,107 +3199,32 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3210,33 +3237,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4101,8 +4101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190:B199"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4165,7 +4165,7 @@
       <c r="Q2" s="166"/>
     </row>
     <row r="3" spans="2:17" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="344" t="s">
+      <c r="B3" s="317" t="s">
         <v>160</v>
       </c>
       <c r="C3" s="145" t="s">
@@ -4190,7 +4190,7 @@
       <c r="Q3" s="166"/>
     </row>
     <row r="4" spans="2:17" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="345"/>
+      <c r="B4" s="318"/>
       <c r="C4" s="243" t="s">
         <v>248</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="Q4" s="166"/>
     </row>
     <row r="5" spans="2:17" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="346"/>
+      <c r="B5" s="319"/>
       <c r="C5" s="106" t="s">
         <v>105</v>
       </c>
@@ -4238,7 +4238,7 @@
       <c r="Q5" s="166"/>
     </row>
     <row r="6" spans="2:17" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="346"/>
+      <c r="B6" s="319"/>
       <c r="C6" s="109" t="s">
         <v>106</v>
       </c>
@@ -4261,7 +4261,7 @@
       <c r="Q6" s="166"/>
     </row>
     <row r="7" spans="2:17" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="347"/>
+      <c r="B7" s="320"/>
       <c r="C7" s="151" t="s">
         <v>154</v>
       </c>
@@ -4286,7 +4286,7 @@
       <c r="Q7" s="166"/>
     </row>
     <row r="8" spans="2:17" ht="14" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="348"/>
+      <c r="B8" s="321"/>
       <c r="C8" s="151" t="s">
         <v>132</v>
       </c>
@@ -4326,7 +4326,7 @@
       <c r="Q9" s="166"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="344" t="s">
+      <c r="B10" s="317" t="s">
         <v>159</v>
       </c>
       <c r="C10" s="244" t="s">
@@ -4353,7 +4353,7 @@
       <c r="Q10" s="166"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="345"/>
+      <c r="B11" s="318"/>
       <c r="C11" s="150" t="s">
         <v>184</v>
       </c>
@@ -4378,7 +4378,7 @@
       <c r="Q11" s="166"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="346"/>
+      <c r="B12" s="319"/>
       <c r="C12" s="301" t="s">
         <v>182</v>
       </c>
@@ -4403,7 +4403,7 @@
       <c r="Q12" s="166"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="346"/>
+      <c r="B13" s="319"/>
       <c r="C13" s="301" t="s">
         <v>183</v>
       </c>
@@ -4426,7 +4426,7 @@
       <c r="Q13" s="166"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="346"/>
+      <c r="B14" s="319"/>
       <c r="C14" s="106" t="s">
         <v>100</v>
       </c>
@@ -4456,7 +4456,7 @@
       <c r="Q14" s="166"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="346"/>
+      <c r="B15" s="319"/>
       <c r="C15" s="106" t="s">
         <v>185</v>
       </c>
@@ -4486,7 +4486,7 @@
       <c r="Q15" s="166"/>
     </row>
     <row r="16" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="347"/>
+      <c r="B16" s="320"/>
       <c r="C16" s="158" t="s">
         <v>109</v>
       </c>
@@ -4535,7 +4535,7 @@
       <c r="Q17" s="166"/>
     </row>
     <row r="18" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="350" t="s">
+      <c r="B18" s="323" t="s">
         <v>194</v>
       </c>
       <c r="C18" s="145" t="s">
@@ -4566,7 +4566,7 @@
       <c r="Q18" s="166"/>
     </row>
     <row r="19" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="351"/>
+      <c r="B19" s="324"/>
       <c r="C19" s="106" t="s">
         <v>156</v>
       </c>
@@ -4593,7 +4593,7 @@
       <c r="Q19" s="166"/>
     </row>
     <row r="20" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="351"/>
+      <c r="B20" s="324"/>
       <c r="C20" s="106" t="s">
         <v>157</v>
       </c>
@@ -4620,7 +4620,7 @@
       <c r="Q20" s="166"/>
     </row>
     <row r="21" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="351"/>
+      <c r="B21" s="324"/>
       <c r="C21" s="158" t="s">
         <v>158</v>
       </c>
@@ -4667,7 +4667,7 @@
       <c r="Q22" s="166"/>
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="352" t="s">
+      <c r="B23" s="325" t="s">
         <v>210</v>
       </c>
       <c r="C23" s="193" t="s">
@@ -4685,12 +4685,12 @@
       <c r="I23" s="230"/>
       <c r="J23" s="231"/>
       <c r="N23" s="164"/>
-      <c r="O23" s="349"/>
-      <c r="P23" s="349"/>
-      <c r="Q23" s="349"/>
+      <c r="O23" s="322"/>
+      <c r="P23" s="322"/>
+      <c r="Q23" s="322"/>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="352"/>
+      <c r="B24" s="325"/>
       <c r="C24" s="194" t="s">
         <v>1</v>
       </c>
@@ -4711,10 +4711,10 @@
       <c r="Q24" s="164"/>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="343" t="s">
+      <c r="A25" s="316" t="s">
         <v>221</v>
       </c>
-      <c r="B25" s="352"/>
+      <c r="B25" s="325"/>
       <c r="C25" s="194" t="s">
         <v>96</v>
       </c>
@@ -4735,8 +4735,8 @@
       <c r="Q25" s="164"/>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="343"/>
-      <c r="B26" s="352"/>
+      <c r="A26" s="316"/>
+      <c r="B26" s="325"/>
       <c r="C26" s="194" t="s">
         <v>2</v>
       </c>
@@ -4757,7 +4757,7 @@
       <c r="Q26" s="164"/>
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="352"/>
+      <c r="B27" s="325"/>
       <c r="C27" s="194" t="s">
         <v>188</v>
       </c>
@@ -4778,7 +4778,7 @@
       <c r="Q27" s="164"/>
     </row>
     <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="352"/>
+      <c r="B28" s="325"/>
       <c r="C28" s="194" t="s">
         <v>69</v>
       </c>
@@ -4799,7 +4799,7 @@
       <c r="Q28" s="164"/>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="352"/>
+      <c r="B29" s="325"/>
       <c r="C29" s="194" t="s">
         <v>33</v>
       </c>
@@ -4820,7 +4820,7 @@
       <c r="Q29" s="164"/>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="352"/>
+      <c r="B30" s="325"/>
       <c r="C30" s="194" t="s">
         <v>163</v>
       </c>
@@ -4841,7 +4841,7 @@
       <c r="Q30" s="164"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="352"/>
+      <c r="B31" s="325"/>
       <c r="C31" s="194" t="s">
         <v>70</v>
       </c>
@@ -4862,7 +4862,7 @@
       <c r="Q31" s="164"/>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="352"/>
+      <c r="B32" s="325"/>
       <c r="C32" s="194" t="s">
         <v>185</v>
       </c>
@@ -4883,7 +4883,7 @@
       <c r="Q32" s="164"/>
     </row>
     <row r="33" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="352"/>
+      <c r="B33" s="325"/>
       <c r="C33" s="195" t="s">
         <v>197</v>
       </c>
@@ -4904,7 +4904,7 @@
       <c r="Q33" s="164"/>
     </row>
     <row r="34" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="352"/>
+      <c r="B34" s="325"/>
       <c r="C34" s="196" t="s">
         <v>136</v>
       </c>
@@ -4925,7 +4925,7 @@
       <c r="Q34" s="164"/>
     </row>
     <row r="35" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="352"/>
+      <c r="B35" s="325"/>
       <c r="C35" s="194" t="s">
         <v>239</v>
       </c>
@@ -4946,7 +4946,7 @@
       <c r="Q35" s="164"/>
     </row>
     <row r="36" spans="2:17" s="310" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="352"/>
+      <c r="B36" s="325"/>
       <c r="C36" s="313" t="s">
         <v>244</v>
       </c>
@@ -4970,7 +4970,7 @@
       <c r="Q36" s="311"/>
     </row>
     <row r="37" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="352"/>
+      <c r="B37" s="325"/>
       <c r="C37" s="197" t="s">
         <v>198</v>
       </c>
@@ -4991,7 +4991,7 @@
       <c r="Q37" s="164"/>
     </row>
     <row r="38" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="352"/>
+      <c r="B38" s="325"/>
       <c r="C38" s="196" t="s">
         <v>199</v>
       </c>
@@ -5012,7 +5012,7 @@
       <c r="Q38" s="164"/>
     </row>
     <row r="39" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="352"/>
+      <c r="B39" s="325"/>
       <c r="C39" s="196" t="s">
         <v>200</v>
       </c>
@@ -5033,7 +5033,7 @@
       <c r="Q39" s="164"/>
     </row>
     <row r="40" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="352"/>
+      <c r="B40" s="325"/>
       <c r="C40" s="196" t="s">
         <v>201</v>
       </c>
@@ -5054,7 +5054,7 @@
       <c r="Q40" s="164"/>
     </row>
     <row r="41" spans="2:17" s="310" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="352"/>
+      <c r="B41" s="325"/>
       <c r="C41" s="302" t="s">
         <v>203</v>
       </c>
@@ -5080,7 +5080,7 @@
       <c r="Q41" s="311"/>
     </row>
     <row r="42" spans="2:17" s="310" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="352"/>
+      <c r="B42" s="325"/>
       <c r="C42" s="302" t="s">
         <v>33</v>
       </c>
@@ -5104,7 +5104,7 @@
       <c r="Q42" s="311"/>
     </row>
     <row r="43" spans="2:17" s="310" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="352"/>
+      <c r="B43" s="325"/>
       <c r="C43" s="302" t="s">
         <v>202</v>
       </c>
@@ -5128,7 +5128,7 @@
       <c r="Q43" s="311"/>
     </row>
     <row r="44" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="352"/>
+      <c r="B44" s="325"/>
       <c r="C44" s="196" t="s">
         <v>204</v>
       </c>
@@ -5149,7 +5149,7 @@
       <c r="Q44" s="164"/>
     </row>
     <row r="45" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="352"/>
+      <c r="B45" s="325"/>
       <c r="C45" s="196" t="s">
         <v>4</v>
       </c>
@@ -5170,7 +5170,7 @@
       <c r="Q45" s="164"/>
     </row>
     <row r="46" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="352"/>
+      <c r="B46" s="325"/>
       <c r="C46" s="196" t="s">
         <v>65</v>
       </c>
@@ -5191,7 +5191,7 @@
       <c r="Q46" s="164"/>
     </row>
     <row r="47" spans="2:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="352"/>
+      <c r="B47" s="325"/>
       <c r="C47" s="198" t="s">
         <v>205</v>
       </c>
@@ -5227,13 +5227,13 @@
       </c>
     </row>
     <row r="49" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="338" t="s">
+      <c r="B49" s="332" t="s">
         <v>247</v>
       </c>
       <c r="C49" s="205" t="s">
         <v>241</v>
       </c>
-      <c r="D49" s="340" t="s">
+      <c r="D49" s="334" t="s">
         <v>246</v>
       </c>
       <c r="E49" s="206"/>
@@ -5255,11 +5255,11 @@
       <c r="Q49" s="90"/>
     </row>
     <row r="50" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="339"/>
+      <c r="B50" s="333"/>
       <c r="C50" s="170" t="s">
         <v>99</v>
       </c>
-      <c r="D50" s="341"/>
+      <c r="D50" s="335"/>
       <c r="E50" s="175"/>
       <c r="F50" s="176"/>
       <c r="G50" s="176"/>
@@ -5278,11 +5278,11 @@
       <c r="Q50" s="90"/>
     </row>
     <row r="51" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="339"/>
+      <c r="B51" s="333"/>
       <c r="C51" s="170" t="s">
         <v>242</v>
       </c>
-      <c r="D51" s="341"/>
+      <c r="D51" s="335"/>
       <c r="E51" s="175"/>
       <c r="F51" s="176"/>
       <c r="G51" s="176"/>
@@ -5301,11 +5301,11 @@
       <c r="Q51" s="90"/>
     </row>
     <row r="52" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="339"/>
+      <c r="B52" s="333"/>
       <c r="C52" s="170" t="s">
         <v>161</v>
       </c>
-      <c r="D52" s="341"/>
+      <c r="D52" s="335"/>
       <c r="E52" s="175"/>
       <c r="F52" s="176"/>
       <c r="G52" s="176"/>
@@ -5324,11 +5324,11 @@
       <c r="Q52" s="90"/>
     </row>
     <row r="53" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="339"/>
+      <c r="B53" s="333"/>
       <c r="C53" s="170" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="341"/>
+      <c r="D53" s="335"/>
       <c r="E53" s="175"/>
       <c r="F53" s="176"/>
       <c r="G53" s="176"/>
@@ -5341,11 +5341,11 @@
       </c>
     </row>
     <row r="54" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="339"/>
+      <c r="B54" s="333"/>
       <c r="C54" s="170" t="s">
         <v>97</v>
       </c>
-      <c r="D54" s="341"/>
+      <c r="D54" s="335"/>
       <c r="E54" s="175"/>
       <c r="F54" s="176"/>
       <c r="G54" s="176"/>
@@ -5358,9 +5358,9 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="339"/>
+      <c r="B55" s="333"/>
       <c r="C55" s="128"/>
-      <c r="D55" s="341"/>
+      <c r="D55" s="335"/>
       <c r="E55" s="129"/>
       <c r="F55" s="114"/>
       <c r="G55" s="114"/>
@@ -5369,11 +5369,11 @@
       <c r="J55" s="118"/>
     </row>
     <row r="56" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="339"/>
+      <c r="B56" s="333"/>
       <c r="C56" s="170" t="s">
         <v>134</v>
       </c>
-      <c r="D56" s="341"/>
+      <c r="D56" s="335"/>
       <c r="E56" s="175"/>
       <c r="F56" s="176"/>
       <c r="G56" s="176"/>
@@ -5385,11 +5385,11 @@
       <c r="J56" s="180"/>
     </row>
     <row r="57" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="339"/>
+      <c r="B57" s="333"/>
       <c r="C57" s="170" t="s">
         <v>174</v>
       </c>
-      <c r="D57" s="341"/>
+      <c r="D57" s="335"/>
       <c r="E57" s="175"/>
       <c r="F57" s="176"/>
       <c r="G57" s="176"/>
@@ -5401,11 +5401,11 @@
       <c r="J57" s="180"/>
     </row>
     <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="339"/>
+      <c r="B58" s="333"/>
       <c r="C58" s="170" t="s">
         <v>177</v>
       </c>
-      <c r="D58" s="341"/>
+      <c r="D58" s="335"/>
       <c r="E58" s="175"/>
       <c r="F58" s="176"/>
       <c r="G58" s="176"/>
@@ -5417,11 +5417,11 @@
       <c r="J58" s="180"/>
     </row>
     <row r="59" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="339"/>
+      <c r="B59" s="333"/>
       <c r="C59" s="170" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="341"/>
+      <c r="D59" s="335"/>
       <c r="E59" s="175"/>
       <c r="F59" s="176"/>
       <c r="G59" s="176"/>
@@ -5433,9 +5433,9 @@
       <c r="J59" s="180"/>
     </row>
     <row r="60" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="339"/>
+      <c r="B60" s="333"/>
       <c r="C60" s="128"/>
-      <c r="D60" s="341"/>
+      <c r="D60" s="335"/>
       <c r="E60" s="129"/>
       <c r="F60" s="114"/>
       <c r="G60" s="114"/>
@@ -5445,11 +5445,11 @@
       <c r="R60" s="81"/>
     </row>
     <row r="61" spans="2:18" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="339"/>
+      <c r="B61" s="333"/>
       <c r="C61" s="170" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="341"/>
+      <c r="D61" s="335"/>
       <c r="E61" s="181"/>
       <c r="F61" s="182"/>
       <c r="G61" s="182"/>
@@ -5461,11 +5461,11 @@
       <c r="J61" s="180"/>
     </row>
     <row r="62" spans="2:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="339"/>
+      <c r="B62" s="333"/>
       <c r="C62" s="170" t="s">
         <v>175</v>
       </c>
-      <c r="D62" s="341"/>
+      <c r="D62" s="335"/>
       <c r="E62" s="181"/>
       <c r="F62" s="182"/>
       <c r="G62" s="182"/>
@@ -5477,11 +5477,11 @@
       <c r="J62" s="180"/>
     </row>
     <row r="63" spans="2:18" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="339"/>
+      <c r="B63" s="333"/>
       <c r="C63" s="170" t="s">
         <v>142</v>
       </c>
-      <c r="D63" s="341"/>
+      <c r="D63" s="335"/>
       <c r="E63" s="181"/>
       <c r="F63" s="182"/>
       <c r="G63" s="182"/>
@@ -5493,9 +5493,9 @@
       <c r="J63" s="180"/>
     </row>
     <row r="64" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="339"/>
+      <c r="B64" s="333"/>
       <c r="C64" s="128"/>
-      <c r="D64" s="341"/>
+      <c r="D64" s="335"/>
       <c r="E64" s="130"/>
       <c r="F64" s="116"/>
       <c r="G64" s="116"/>
@@ -5504,11 +5504,11 @@
       <c r="J64" s="119"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="339"/>
+      <c r="B65" s="333"/>
       <c r="C65" s="170" t="s">
         <v>176</v>
       </c>
-      <c r="D65" s="341"/>
+      <c r="D65" s="335"/>
       <c r="E65" s="181"/>
       <c r="F65" s="182"/>
       <c r="G65" s="182"/>
@@ -5522,11 +5522,11 @@
       <c r="Q65" s="165"/>
     </row>
     <row r="66" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="339"/>
+      <c r="B66" s="333"/>
       <c r="C66" s="170" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="341"/>
+      <c r="D66" s="335"/>
       <c r="E66" s="181"/>
       <c r="F66" s="182"/>
       <c r="G66" s="182"/>
@@ -5539,11 +5539,11 @@
       <c r="Q66" s="166"/>
     </row>
     <row r="67" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="339"/>
+      <c r="B67" s="333"/>
       <c r="C67" s="171" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="341"/>
+      <c r="D67" s="335"/>
       <c r="E67" s="184"/>
       <c r="F67" s="185"/>
       <c r="G67" s="185"/>
@@ -5557,11 +5557,11 @@
       <c r="Q67" s="90"/>
     </row>
     <row r="68" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="339"/>
+      <c r="B68" s="333"/>
       <c r="C68" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="D68" s="341"/>
+      <c r="D68" s="335"/>
       <c r="E68" s="114"/>
       <c r="F68" s="114"/>
       <c r="G68" s="114"/>
@@ -5574,11 +5574,11 @@
       <c r="Q68" s="90"/>
     </row>
     <row r="69" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="339"/>
+      <c r="B69" s="333"/>
       <c r="C69" s="172" t="s">
         <v>102</v>
       </c>
-      <c r="D69" s="341"/>
+      <c r="D69" s="335"/>
       <c r="E69" s="182"/>
       <c r="F69" s="182"/>
       <c r="G69" s="182"/>
@@ -5591,11 +5591,11 @@
       <c r="Q69" s="90"/>
     </row>
     <row r="70" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="339"/>
+      <c r="B70" s="333"/>
       <c r="C70" s="172" t="s">
         <v>170</v>
       </c>
-      <c r="D70" s="341"/>
+      <c r="D70" s="335"/>
       <c r="E70" s="182"/>
       <c r="F70" s="182"/>
       <c r="G70" s="182"/>
@@ -5608,11 +5608,11 @@
       <c r="Q70" s="90"/>
     </row>
     <row r="71" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="339"/>
+      <c r="B71" s="333"/>
       <c r="C71" s="172" t="s">
         <v>283</v>
       </c>
-      <c r="D71" s="341"/>
+      <c r="D71" s="335"/>
       <c r="E71" s="182"/>
       <c r="F71" s="182"/>
       <c r="G71" s="182"/>
@@ -5623,11 +5623,11 @@
       <c r="J71" s="180"/>
     </row>
     <row r="72" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="339"/>
+      <c r="B72" s="333"/>
       <c r="C72" s="172" t="s">
         <v>284</v>
       </c>
-      <c r="D72" s="341"/>
+      <c r="D72" s="335"/>
       <c r="E72" s="182"/>
       <c r="F72" s="182"/>
       <c r="G72" s="182"/>
@@ -5638,11 +5638,11 @@
       <c r="J72" s="180"/>
     </row>
     <row r="73" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="339"/>
+      <c r="B73" s="333"/>
       <c r="C73" s="172" t="s">
         <v>101</v>
       </c>
-      <c r="D73" s="341"/>
+      <c r="D73" s="335"/>
       <c r="E73" s="182"/>
       <c r="F73" s="182"/>
       <c r="G73" s="182"/>
@@ -5653,11 +5653,11 @@
       <c r="J73" s="180"/>
     </row>
     <row r="74" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="339"/>
+      <c r="B74" s="333"/>
       <c r="C74" s="172" t="s">
         <v>285</v>
       </c>
-      <c r="D74" s="341"/>
+      <c r="D74" s="335"/>
       <c r="E74" s="182"/>
       <c r="F74" s="182"/>
       <c r="G74" s="182"/>
@@ -5668,11 +5668,11 @@
       <c r="J74" s="180"/>
     </row>
     <row r="75" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="339"/>
+      <c r="B75" s="333"/>
       <c r="C75" s="172" t="s">
         <v>299</v>
       </c>
-      <c r="D75" s="341"/>
+      <c r="D75" s="335"/>
       <c r="E75" s="182"/>
       <c r="F75" s="182"/>
       <c r="G75" s="182"/>
@@ -5683,11 +5683,11 @@
       <c r="J75" s="180"/>
     </row>
     <row r="76" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="339"/>
+      <c r="B76" s="333"/>
       <c r="C76" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="D76" s="341"/>
+      <c r="D76" s="335"/>
       <c r="E76" s="182"/>
       <c r="F76" s="182"/>
       <c r="G76" s="182"/>
@@ -5698,11 +5698,11 @@
       <c r="J76" s="180"/>
     </row>
     <row r="77" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="339"/>
+      <c r="B77" s="333"/>
       <c r="C77" s="172" t="s">
         <v>289</v>
       </c>
-      <c r="D77" s="341"/>
+      <c r="D77" s="335"/>
       <c r="E77" s="182"/>
       <c r="F77" s="182"/>
       <c r="G77" s="182"/>
@@ -5713,11 +5713,11 @@
       <c r="J77" s="180"/>
     </row>
     <row r="78" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="339"/>
+      <c r="B78" s="333"/>
       <c r="C78" s="173" t="s">
         <v>290</v>
       </c>
-      <c r="D78" s="341"/>
+      <c r="D78" s="335"/>
       <c r="E78" s="182"/>
       <c r="F78" s="182"/>
       <c r="G78" s="182"/>
@@ -5728,11 +5728,11 @@
       <c r="J78" s="180"/>
     </row>
     <row r="79" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="339"/>
+      <c r="B79" s="333"/>
       <c r="C79" s="173" t="s">
         <v>110</v>
       </c>
-      <c r="D79" s="341"/>
+      <c r="D79" s="335"/>
       <c r="E79" s="182"/>
       <c r="F79" s="182"/>
       <c r="G79" s="182"/>
@@ -5744,11 +5744,11 @@
       <c r="P79" s="101"/>
     </row>
     <row r="80" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="339"/>
+      <c r="B80" s="333"/>
       <c r="C80" s="113" t="s">
         <v>206</v>
       </c>
-      <c r="D80" s="341"/>
+      <c r="D80" s="335"/>
       <c r="E80" s="114"/>
       <c r="F80" s="114"/>
       <c r="G80" s="114"/>
@@ -5757,12 +5757,12 @@
       <c r="J80" s="115"/>
     </row>
     <row r="81" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="339"/>
+      <c r="B81" s="333"/>
       <c r="C81" s="174">
         <f>I18</f>
         <v>0</v>
       </c>
-      <c r="D81" s="341"/>
+      <c r="D81" s="335"/>
       <c r="E81" s="182"/>
       <c r="F81" s="182"/>
       <c r="G81" s="182"/>
@@ -5774,12 +5774,12 @@
       <c r="O81" s="90"/>
     </row>
     <row r="82" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="339"/>
+      <c r="B82" s="333"/>
       <c r="C82" s="174">
         <f>I19</f>
         <v>0</v>
       </c>
-      <c r="D82" s="341"/>
+      <c r="D82" s="335"/>
       <c r="E82" s="182"/>
       <c r="F82" s="182"/>
       <c r="G82" s="182"/>
@@ -5791,12 +5791,12 @@
       <c r="O82" s="90"/>
     </row>
     <row r="83" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="339"/>
+      <c r="B83" s="333"/>
       <c r="C83" s="174">
         <f>I20</f>
         <v>0</v>
       </c>
-      <c r="D83" s="341"/>
+      <c r="D83" s="335"/>
       <c r="E83" s="182"/>
       <c r="F83" s="182"/>
       <c r="G83" s="182"/>
@@ -5809,12 +5809,12 @@
       <c r="P83" s="167"/>
     </row>
     <row r="84" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B84" s="339"/>
+      <c r="B84" s="333"/>
       <c r="C84" s="174">
         <f>I21</f>
         <v>0</v>
       </c>
-      <c r="D84" s="341"/>
+      <c r="D84" s="335"/>
       <c r="E84" s="182"/>
       <c r="F84" s="182"/>
       <c r="G84" s="182"/>
@@ -5829,11 +5829,11 @@
       <c r="T84" s="38"/>
     </row>
     <row r="85" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B85" s="339"/>
+      <c r="B85" s="333"/>
       <c r="C85" s="113" t="s">
         <v>207</v>
       </c>
-      <c r="D85" s="341"/>
+      <c r="D85" s="335"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
       <c r="G85" s="114"/>
@@ -5845,12 +5845,12 @@
       <c r="T85" s="37"/>
     </row>
     <row r="86" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B86" s="339"/>
+      <c r="B86" s="333"/>
       <c r="C86" s="174">
         <f>C81</f>
         <v>0</v>
       </c>
-      <c r="D86" s="341"/>
+      <c r="D86" s="335"/>
       <c r="E86" s="182"/>
       <c r="F86" s="182"/>
       <c r="G86" s="182"/>
@@ -5865,12 +5865,12 @@
       <c r="T86" s="38"/>
     </row>
     <row r="87" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="339"/>
+      <c r="B87" s="333"/>
       <c r="C87" s="174">
         <f>C82</f>
         <v>0</v>
       </c>
-      <c r="D87" s="341"/>
+      <c r="D87" s="335"/>
       <c r="E87" s="182"/>
       <c r="F87" s="182"/>
       <c r="G87" s="182"/>
@@ -5882,12 +5882,12 @@
       <c r="J87" s="177"/>
     </row>
     <row r="88" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="339"/>
+      <c r="B88" s="333"/>
       <c r="C88" s="174">
         <f>C83</f>
         <v>0</v>
       </c>
-      <c r="D88" s="341"/>
+      <c r="D88" s="335"/>
       <c r="E88" s="177"/>
       <c r="F88" s="177"/>
       <c r="G88" s="177"/>
@@ -5899,12 +5899,12 @@
       <c r="J88" s="177"/>
     </row>
     <row r="89" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="339"/>
+      <c r="B89" s="333"/>
       <c r="C89" s="174">
         <f>C84</f>
         <v>0</v>
       </c>
-      <c r="D89" s="341"/>
+      <c r="D89" s="335"/>
       <c r="E89" s="182"/>
       <c r="F89" s="182"/>
       <c r="G89" s="182"/>
@@ -5916,11 +5916,11 @@
       <c r="J89" s="177"/>
     </row>
     <row r="90" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="339"/>
+      <c r="B90" s="333"/>
       <c r="C90" s="113" t="s">
         <v>208</v>
       </c>
-      <c r="D90" s="341"/>
+      <c r="D90" s="335"/>
       <c r="E90" s="114"/>
       <c r="F90" s="114"/>
       <c r="G90" s="114"/>
@@ -5929,12 +5929,12 @@
       <c r="J90" s="115"/>
     </row>
     <row r="91" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="339"/>
+      <c r="B91" s="333"/>
       <c r="C91" s="174">
         <f>C86</f>
         <v>0</v>
       </c>
-      <c r="D91" s="341"/>
+      <c r="D91" s="335"/>
       <c r="E91" s="182"/>
       <c r="F91" s="182"/>
       <c r="G91" s="182"/>
@@ -5945,12 +5945,12 @@
       <c r="J91" s="177"/>
     </row>
     <row r="92" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="339"/>
+      <c r="B92" s="333"/>
       <c r="C92" s="174">
         <f>C87</f>
         <v>0</v>
       </c>
-      <c r="D92" s="341"/>
+      <c r="D92" s="335"/>
       <c r="E92" s="182"/>
       <c r="F92" s="182"/>
       <c r="G92" s="182"/>
@@ -5961,12 +5961,12 @@
       <c r="J92" s="177"/>
     </row>
     <row r="93" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="339"/>
+      <c r="B93" s="333"/>
       <c r="C93" s="174">
         <f>C88</f>
         <v>0</v>
       </c>
-      <c r="D93" s="341"/>
+      <c r="D93" s="335"/>
       <c r="E93" s="182"/>
       <c r="F93" s="182"/>
       <c r="G93" s="182"/>
@@ -5977,12 +5977,12 @@
       <c r="J93" s="177"/>
     </row>
     <row r="94" spans="2:20" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="339"/>
+      <c r="B94" s="333"/>
       <c r="C94" s="174">
         <f>C89</f>
         <v>0</v>
       </c>
-      <c r="D94" s="342"/>
+      <c r="D94" s="336"/>
       <c r="E94" s="182"/>
       <c r="F94" s="182"/>
       <c r="G94" s="182"/>
@@ -6019,7 +6019,7 @@
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B99" s="324" t="s">
+      <c r="B99" s="326" t="s">
         <v>102</v>
       </c>
       <c r="C99" s="265">
@@ -6027,95 +6027,98 @@
       </c>
       <c r="D99" s="266"/>
       <c r="E99" s="267"/>
-      <c r="F99" s="337"/>
+      <c r="F99" s="329">
+        <f>SUM(E99:E108)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B100" s="319"/>
+      <c r="B100" s="327"/>
       <c r="C100" s="268">
         <v>2</v>
       </c>
       <c r="D100" s="240"/>
       <c r="E100" s="269"/>
-      <c r="F100" s="329"/>
+      <c r="F100" s="330"/>
     </row>
     <row r="101" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="319"/>
+      <c r="B101" s="327"/>
       <c r="C101" s="268">
         <v>3</v>
       </c>
       <c r="D101" s="240"/>
       <c r="E101" s="269"/>
-      <c r="F101" s="329"/>
+      <c r="F101" s="330"/>
     </row>
     <row r="102" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="319"/>
+      <c r="B102" s="327"/>
       <c r="C102" s="268">
         <v>4</v>
       </c>
       <c r="D102" s="240"/>
       <c r="E102" s="269"/>
-      <c r="F102" s="329"/>
+      <c r="F102" s="330"/>
       <c r="G102" s="102"/>
       <c r="H102" s="88"/>
       <c r="I102" s="102"/>
       <c r="J102" s="88"/>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B103" s="319"/>
+      <c r="B103" s="327"/>
       <c r="C103" s="268">
         <v>5</v>
       </c>
       <c r="D103" s="240"/>
       <c r="E103" s="269"/>
-      <c r="F103" s="329"/>
+      <c r="F103" s="330"/>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B104" s="319"/>
+      <c r="B104" s="327"/>
       <c r="C104" s="268">
         <v>6</v>
       </c>
       <c r="D104" s="240"/>
       <c r="E104" s="269"/>
-      <c r="F104" s="329"/>
+      <c r="F104" s="330"/>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B105" s="319"/>
+      <c r="B105" s="327"/>
       <c r="C105" s="268">
         <v>7</v>
       </c>
       <c r="D105" s="240"/>
       <c r="E105" s="269"/>
-      <c r="F105" s="329"/>
+      <c r="F105" s="330"/>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B106" s="319"/>
+      <c r="B106" s="327"/>
       <c r="C106" s="268">
         <v>8</v>
       </c>
       <c r="D106" s="240"/>
       <c r="E106" s="269"/>
-      <c r="F106" s="329"/>
+      <c r="F106" s="330"/>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B107" s="319"/>
+      <c r="B107" s="327"/>
       <c r="C107" s="268">
         <v>9</v>
       </c>
       <c r="D107" s="240"/>
       <c r="E107" s="269"/>
-      <c r="F107" s="329"/>
+      <c r="F107" s="330"/>
     </row>
     <row r="108" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="320"/>
+      <c r="B108" s="328"/>
       <c r="C108" s="270">
         <v>10</v>
       </c>
       <c r="D108" s="271"/>
       <c r="E108" s="272"/>
-      <c r="F108" s="330"/>
+      <c r="F108" s="331"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B109" s="324" t="s">
+      <c r="B109" s="326" t="s">
         <v>170</v>
       </c>
       <c r="C109" s="265">
@@ -6123,94 +6126,94 @@
       </c>
       <c r="D109" s="266"/>
       <c r="E109" s="273"/>
-      <c r="F109" s="328">
+      <c r="F109" s="337">
         <f>SUM(E109:E118)</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B110" s="319"/>
+      <c r="B110" s="327"/>
       <c r="C110" s="268">
         <v>2</v>
       </c>
       <c r="D110" s="240"/>
       <c r="E110" s="269"/>
-      <c r="F110" s="329"/>
+      <c r="F110" s="330"/>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B111" s="319"/>
+      <c r="B111" s="327"/>
       <c r="C111" s="268">
         <v>3</v>
       </c>
       <c r="D111" s="240"/>
       <c r="E111" s="269"/>
-      <c r="F111" s="329"/>
+      <c r="F111" s="330"/>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B112" s="319"/>
+      <c r="B112" s="327"/>
       <c r="C112" s="268">
         <v>4</v>
       </c>
       <c r="D112" s="240"/>
       <c r="E112" s="269"/>
-      <c r="F112" s="329"/>
+      <c r="F112" s="330"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B113" s="319"/>
+      <c r="B113" s="327"/>
       <c r="C113" s="268">
         <v>5</v>
       </c>
       <c r="D113" s="240"/>
       <c r="E113" s="269"/>
-      <c r="F113" s="329"/>
+      <c r="F113" s="330"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B114" s="319"/>
+      <c r="B114" s="327"/>
       <c r="C114" s="268">
         <v>6</v>
       </c>
       <c r="D114" s="240"/>
       <c r="E114" s="269"/>
-      <c r="F114" s="329"/>
+      <c r="F114" s="330"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B115" s="319"/>
+      <c r="B115" s="327"/>
       <c r="C115" s="268">
         <v>7</v>
       </c>
       <c r="D115" s="240"/>
       <c r="E115" s="269"/>
-      <c r="F115" s="329"/>
+      <c r="F115" s="330"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B116" s="319"/>
+      <c r="B116" s="327"/>
       <c r="C116" s="268">
         <v>8</v>
       </c>
       <c r="D116" s="240"/>
       <c r="E116" s="269"/>
-      <c r="F116" s="329"/>
+      <c r="F116" s="330"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B117" s="319"/>
+      <c r="B117" s="327"/>
       <c r="C117" s="268">
         <v>9</v>
       </c>
       <c r="D117" s="240"/>
       <c r="E117" s="269"/>
-      <c r="F117" s="329"/>
+      <c r="F117" s="330"/>
     </row>
     <row r="118" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="320"/>
+      <c r="B118" s="328"/>
       <c r="C118" s="270">
         <v>10</v>
       </c>
       <c r="D118" s="271"/>
       <c r="E118" s="272"/>
-      <c r="F118" s="330"/>
+      <c r="F118" s="331"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B119" s="324" t="s">
+      <c r="B119" s="326" t="s">
         <v>283</v>
       </c>
       <c r="C119" s="265">
@@ -6218,94 +6221,94 @@
       </c>
       <c r="D119" s="266"/>
       <c r="E119" s="273"/>
-      <c r="F119" s="328">
+      <c r="F119" s="337">
         <f>SUM(E119:E128)</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B120" s="319"/>
+      <c r="B120" s="327"/>
       <c r="C120" s="268">
         <v>2</v>
       </c>
       <c r="D120" s="240"/>
       <c r="E120" s="269"/>
-      <c r="F120" s="329"/>
+      <c r="F120" s="330"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B121" s="319"/>
+      <c r="B121" s="327"/>
       <c r="C121" s="268">
         <v>3</v>
       </c>
       <c r="D121" s="240"/>
       <c r="E121" s="269"/>
-      <c r="F121" s="329"/>
+      <c r="F121" s="330"/>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B122" s="319"/>
+      <c r="B122" s="327"/>
       <c r="C122" s="268">
         <v>4</v>
       </c>
       <c r="D122" s="240"/>
       <c r="E122" s="269"/>
-      <c r="F122" s="329"/>
+      <c r="F122" s="330"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B123" s="319"/>
+      <c r="B123" s="327"/>
       <c r="C123" s="268">
         <v>5</v>
       </c>
       <c r="D123" s="240"/>
       <c r="E123" s="269"/>
-      <c r="F123" s="329"/>
+      <c r="F123" s="330"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B124" s="319"/>
+      <c r="B124" s="327"/>
       <c r="C124" s="268">
         <v>6</v>
       </c>
       <c r="D124" s="240"/>
       <c r="E124" s="269"/>
-      <c r="F124" s="329"/>
+      <c r="F124" s="330"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B125" s="319"/>
+      <c r="B125" s="327"/>
       <c r="C125" s="268">
         <v>7</v>
       </c>
       <c r="D125" s="240"/>
       <c r="E125" s="269"/>
-      <c r="F125" s="329"/>
+      <c r="F125" s="330"/>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B126" s="319"/>
+      <c r="B126" s="327"/>
       <c r="C126" s="268">
         <v>8</v>
       </c>
       <c r="D126" s="240"/>
       <c r="E126" s="269"/>
-      <c r="F126" s="329"/>
+      <c r="F126" s="330"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B127" s="319"/>
+      <c r="B127" s="327"/>
       <c r="C127" s="268">
         <v>9</v>
       </c>
       <c r="D127" s="240"/>
       <c r="E127" s="269"/>
-      <c r="F127" s="329"/>
+      <c r="F127" s="330"/>
     </row>
     <row r="128" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="320"/>
+      <c r="B128" s="328"/>
       <c r="C128" s="270">
         <v>10</v>
       </c>
       <c r="D128" s="271"/>
       <c r="E128" s="272"/>
-      <c r="F128" s="330"/>
+      <c r="F128" s="331"/>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B129" s="324" t="s">
+      <c r="B129" s="326" t="s">
         <v>284</v>
       </c>
       <c r="C129" s="265">
@@ -6313,31 +6316,31 @@
       </c>
       <c r="D129" s="266"/>
       <c r="E129" s="273"/>
-      <c r="F129" s="328">
+      <c r="F129" s="337">
         <f>SUM(E129:E131)</f>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B130" s="319"/>
+      <c r="B130" s="327"/>
       <c r="C130" s="268">
         <v>2</v>
       </c>
       <c r="D130" s="240"/>
       <c r="E130" s="269"/>
-      <c r="F130" s="329"/>
+      <c r="F130" s="330"/>
     </row>
     <row r="131" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B131" s="319"/>
+      <c r="B131" s="327"/>
       <c r="C131" s="268">
         <v>3</v>
       </c>
       <c r="D131" s="240"/>
       <c r="E131" s="269"/>
-      <c r="F131" s="329"/>
+      <c r="F131" s="330"/>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B132" s="325" t="s">
+      <c r="B132" s="338" t="s">
         <v>285</v>
       </c>
       <c r="C132" s="274">
@@ -6345,85 +6348,85 @@
       </c>
       <c r="D132" s="275"/>
       <c r="E132" s="276"/>
-      <c r="F132" s="334">
+      <c r="F132" s="341">
         <f>SUM(E132:E140)</f>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B133" s="326"/>
+      <c r="B133" s="339"/>
       <c r="C133" s="277">
         <v>2</v>
       </c>
       <c r="D133" s="278"/>
       <c r="E133" s="279"/>
-      <c r="F133" s="335"/>
+      <c r="F133" s="342"/>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B134" s="326"/>
+      <c r="B134" s="339"/>
       <c r="C134" s="277">
         <v>3</v>
       </c>
       <c r="D134" s="278"/>
       <c r="E134" s="279"/>
-      <c r="F134" s="335"/>
+      <c r="F134" s="342"/>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B135" s="326"/>
+      <c r="B135" s="339"/>
       <c r="C135" s="277">
         <v>4</v>
       </c>
       <c r="D135" s="278"/>
       <c r="E135" s="279"/>
-      <c r="F135" s="335"/>
+      <c r="F135" s="342"/>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B136" s="326"/>
+      <c r="B136" s="339"/>
       <c r="C136" s="277">
         <v>5</v>
       </c>
       <c r="D136" s="278"/>
       <c r="E136" s="279"/>
-      <c r="F136" s="335"/>
+      <c r="F136" s="342"/>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B137" s="326"/>
+      <c r="B137" s="339"/>
       <c r="C137" s="277">
         <v>6</v>
       </c>
       <c r="D137" s="278"/>
       <c r="E137" s="279"/>
-      <c r="F137" s="335"/>
+      <c r="F137" s="342"/>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B138" s="326"/>
+      <c r="B138" s="339"/>
       <c r="C138" s="277">
         <v>7</v>
       </c>
       <c r="D138" s="278"/>
       <c r="E138" s="279"/>
-      <c r="F138" s="335"/>
+      <c r="F138" s="342"/>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B139" s="326"/>
+      <c r="B139" s="339"/>
       <c r="C139" s="234">
         <v>8</v>
       </c>
       <c r="D139" s="280"/>
       <c r="E139" s="281"/>
-      <c r="F139" s="335"/>
+      <c r="F139" s="342"/>
     </row>
     <row r="140" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="327"/>
+      <c r="B140" s="340"/>
       <c r="C140" s="282">
         <v>9</v>
       </c>
       <c r="D140" s="283"/>
       <c r="E140" s="284"/>
-      <c r="F140" s="336"/>
+      <c r="F140" s="343"/>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B141" s="324" t="s">
+      <c r="B141" s="326" t="s">
         <v>286</v>
       </c>
       <c r="C141" s="285">
@@ -6431,94 +6434,94 @@
       </c>
       <c r="D141" s="286"/>
       <c r="E141" s="287"/>
-      <c r="F141" s="328">
+      <c r="F141" s="337">
         <f>SUM(E141:E150)</f>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B142" s="319"/>
+      <c r="B142" s="327"/>
       <c r="C142" s="268">
         <v>2</v>
       </c>
       <c r="D142" s="240"/>
       <c r="E142" s="269"/>
-      <c r="F142" s="329"/>
+      <c r="F142" s="330"/>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B143" s="319"/>
+      <c r="B143" s="327"/>
       <c r="C143" s="268">
         <v>3</v>
       </c>
       <c r="D143" s="240"/>
       <c r="E143" s="269"/>
-      <c r="F143" s="329"/>
+      <c r="F143" s="330"/>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B144" s="319"/>
+      <c r="B144" s="327"/>
       <c r="C144" s="268">
         <v>4</v>
       </c>
       <c r="D144" s="240"/>
       <c r="E144" s="269"/>
-      <c r="F144" s="329"/>
+      <c r="F144" s="330"/>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B145" s="319"/>
+      <c r="B145" s="327"/>
       <c r="C145" s="268">
         <v>5</v>
       </c>
       <c r="D145" s="240"/>
       <c r="E145" s="269"/>
-      <c r="F145" s="329"/>
+      <c r="F145" s="330"/>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B146" s="319"/>
+      <c r="B146" s="327"/>
       <c r="C146" s="268">
         <v>6</v>
       </c>
       <c r="D146" s="240"/>
       <c r="E146" s="269"/>
-      <c r="F146" s="329"/>
+      <c r="F146" s="330"/>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B147" s="319"/>
+      <c r="B147" s="327"/>
       <c r="C147" s="268">
         <v>7</v>
       </c>
       <c r="D147" s="240"/>
       <c r="E147" s="269"/>
-      <c r="F147" s="329"/>
+      <c r="F147" s="330"/>
     </row>
     <row r="148" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B148" s="319"/>
+      <c r="B148" s="327"/>
       <c r="C148" s="268">
         <v>8</v>
       </c>
       <c r="D148" s="240"/>
       <c r="E148" s="269"/>
-      <c r="F148" s="329"/>
+      <c r="F148" s="330"/>
     </row>
     <row r="149" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B149" s="319"/>
+      <c r="B149" s="327"/>
       <c r="C149" s="268">
         <v>9</v>
       </c>
       <c r="D149" s="240"/>
       <c r="E149" s="269"/>
-      <c r="F149" s="329"/>
+      <c r="F149" s="330"/>
     </row>
     <row r="150" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="320"/>
+      <c r="B150" s="328"/>
       <c r="C150" s="288">
         <v>10</v>
       </c>
       <c r="D150" s="241"/>
       <c r="E150" s="289"/>
-      <c r="F150" s="330"/>
+      <c r="F150" s="331"/>
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B151" s="324" t="s">
+      <c r="B151" s="326" t="s">
         <v>287</v>
       </c>
       <c r="C151" s="290">
@@ -6526,94 +6529,94 @@
       </c>
       <c r="D151" s="266"/>
       <c r="E151" s="291"/>
-      <c r="F151" s="331">
+      <c r="F151" s="344">
         <f>SUM(E151:E160)</f>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B152" s="319"/>
+      <c r="B152" s="327"/>
       <c r="C152" s="292">
         <v>2</v>
       </c>
       <c r="D152" s="240"/>
       <c r="E152" s="293"/>
-      <c r="F152" s="332"/>
+      <c r="F152" s="345"/>
     </row>
     <row r="153" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B153" s="319"/>
+      <c r="B153" s="327"/>
       <c r="C153" s="292">
         <v>3</v>
       </c>
       <c r="D153" s="240"/>
       <c r="E153" s="293"/>
-      <c r="F153" s="332"/>
+      <c r="F153" s="345"/>
     </row>
     <row r="154" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B154" s="319"/>
+      <c r="B154" s="327"/>
       <c r="C154" s="292">
         <v>4</v>
       </c>
       <c r="D154" s="240"/>
       <c r="E154" s="293"/>
-      <c r="F154" s="332"/>
+      <c r="F154" s="345"/>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B155" s="319"/>
+      <c r="B155" s="327"/>
       <c r="C155" s="292">
         <v>5</v>
       </c>
       <c r="D155" s="240"/>
       <c r="E155" s="293"/>
-      <c r="F155" s="332"/>
+      <c r="F155" s="345"/>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B156" s="319"/>
+      <c r="B156" s="327"/>
       <c r="C156" s="292">
         <v>6</v>
       </c>
       <c r="D156" s="240"/>
       <c r="E156" s="293"/>
-      <c r="F156" s="332"/>
+      <c r="F156" s="345"/>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B157" s="319"/>
+      <c r="B157" s="327"/>
       <c r="C157" s="292">
         <v>7</v>
       </c>
       <c r="D157" s="240"/>
       <c r="E157" s="293"/>
-      <c r="F157" s="332"/>
+      <c r="F157" s="345"/>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B158" s="319"/>
+      <c r="B158" s="327"/>
       <c r="C158" s="292">
         <v>8</v>
       </c>
       <c r="D158" s="240"/>
       <c r="E158" s="293"/>
-      <c r="F158" s="332"/>
+      <c r="F158" s="345"/>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B159" s="319"/>
+      <c r="B159" s="327"/>
       <c r="C159" s="292">
         <v>9</v>
       </c>
       <c r="D159" s="240"/>
       <c r="E159" s="293"/>
-      <c r="F159" s="332"/>
+      <c r="F159" s="345"/>
     </row>
     <row r="160" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="320"/>
+      <c r="B160" s="328"/>
       <c r="C160" s="294">
         <v>10</v>
       </c>
       <c r="D160" s="271"/>
       <c r="E160" s="295"/>
-      <c r="F160" s="333"/>
+      <c r="F160" s="346"/>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B161" s="319" t="s">
+      <c r="B161" s="327" t="s">
         <v>288</v>
       </c>
       <c r="C161" s="290">
@@ -6621,94 +6624,94 @@
       </c>
       <c r="D161" s="266"/>
       <c r="E161" s="273"/>
-      <c r="F161" s="321">
+      <c r="F161" s="347">
         <f>SUM(E161:E170)</f>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B162" s="319"/>
+      <c r="B162" s="327"/>
       <c r="C162" s="292">
         <v>2</v>
       </c>
       <c r="D162" s="240"/>
       <c r="E162" s="269"/>
-      <c r="F162" s="322"/>
+      <c r="F162" s="348"/>
     </row>
     <row r="163" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B163" s="319"/>
+      <c r="B163" s="327"/>
       <c r="C163" s="292">
         <v>3</v>
       </c>
       <c r="D163" s="240"/>
       <c r="E163" s="269"/>
-      <c r="F163" s="322"/>
+      <c r="F163" s="348"/>
     </row>
     <row r="164" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B164" s="319"/>
+      <c r="B164" s="327"/>
       <c r="C164" s="292">
         <v>4</v>
       </c>
       <c r="D164" s="240"/>
       <c r="E164" s="269"/>
-      <c r="F164" s="322"/>
+      <c r="F164" s="348"/>
     </row>
     <row r="165" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B165" s="319"/>
+      <c r="B165" s="327"/>
       <c r="C165" s="292">
         <v>5</v>
       </c>
       <c r="D165" s="240"/>
       <c r="E165" s="269"/>
-      <c r="F165" s="322"/>
+      <c r="F165" s="348"/>
     </row>
     <row r="166" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B166" s="319"/>
+      <c r="B166" s="327"/>
       <c r="C166" s="292">
         <v>6</v>
       </c>
       <c r="D166" s="240"/>
       <c r="E166" s="269"/>
-      <c r="F166" s="322"/>
+      <c r="F166" s="348"/>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B167" s="319"/>
+      <c r="B167" s="327"/>
       <c r="C167" s="292">
         <v>7</v>
       </c>
       <c r="D167" s="240"/>
       <c r="E167" s="269"/>
-      <c r="F167" s="322"/>
+      <c r="F167" s="348"/>
     </row>
     <row r="168" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B168" s="319"/>
+      <c r="B168" s="327"/>
       <c r="C168" s="292">
         <v>8</v>
       </c>
       <c r="D168" s="240"/>
       <c r="E168" s="269"/>
-      <c r="F168" s="322"/>
+      <c r="F168" s="348"/>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B169" s="319"/>
+      <c r="B169" s="327"/>
       <c r="C169" s="292">
         <v>9</v>
       </c>
       <c r="D169" s="240"/>
       <c r="E169" s="269"/>
-      <c r="F169" s="322"/>
+      <c r="F169" s="348"/>
     </row>
     <row r="170" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B170" s="320"/>
+      <c r="B170" s="328"/>
       <c r="C170" s="294">
         <v>10</v>
       </c>
       <c r="D170" s="271"/>
       <c r="E170" s="272"/>
-      <c r="F170" s="323"/>
+      <c r="F170" s="349"/>
     </row>
     <row r="171" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B171" s="324" t="s">
+      <c r="B171" s="326" t="s">
         <v>289</v>
       </c>
       <c r="C171" s="285">
@@ -6716,85 +6719,85 @@
       </c>
       <c r="D171" s="286"/>
       <c r="E171" s="287"/>
-      <c r="F171" s="321">
+      <c r="F171" s="347">
         <f>SUM(E171:E179)</f>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B172" s="319"/>
+      <c r="B172" s="327"/>
       <c r="C172" s="268">
         <v>2</v>
       </c>
       <c r="D172" s="240"/>
       <c r="E172" s="269"/>
-      <c r="F172" s="322"/>
+      <c r="F172" s="348"/>
     </row>
     <row r="173" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B173" s="319"/>
+      <c r="B173" s="327"/>
       <c r="C173" s="268">
         <v>3</v>
       </c>
       <c r="D173" s="240"/>
       <c r="E173" s="269"/>
-      <c r="F173" s="322"/>
+      <c r="F173" s="348"/>
     </row>
     <row r="174" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B174" s="319"/>
+      <c r="B174" s="327"/>
       <c r="C174" s="268">
         <v>4</v>
       </c>
       <c r="D174" s="240"/>
       <c r="E174" s="269"/>
-      <c r="F174" s="322"/>
+      <c r="F174" s="348"/>
     </row>
     <row r="175" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B175" s="319"/>
+      <c r="B175" s="327"/>
       <c r="C175" s="268">
         <v>5</v>
       </c>
       <c r="D175" s="240"/>
       <c r="E175" s="269"/>
-      <c r="F175" s="322"/>
+      <c r="F175" s="348"/>
     </row>
     <row r="176" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B176" s="319"/>
+      <c r="B176" s="327"/>
       <c r="C176" s="268">
         <v>6</v>
       </c>
       <c r="D176" s="240"/>
       <c r="E176" s="269"/>
-      <c r="F176" s="322"/>
+      <c r="F176" s="348"/>
     </row>
     <row r="177" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B177" s="319"/>
+      <c r="B177" s="327"/>
       <c r="C177" s="268">
         <v>7</v>
       </c>
       <c r="D177" s="240"/>
       <c r="E177" s="269"/>
-      <c r="F177" s="322"/>
+      <c r="F177" s="348"/>
     </row>
     <row r="178" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B178" s="319"/>
+      <c r="B178" s="327"/>
       <c r="C178" s="268">
         <v>8</v>
       </c>
       <c r="D178" s="240"/>
       <c r="E178" s="269"/>
-      <c r="F178" s="322"/>
+      <c r="F178" s="348"/>
     </row>
     <row r="179" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B179" s="319"/>
+      <c r="B179" s="327"/>
       <c r="C179" s="288">
         <v>9</v>
       </c>
       <c r="D179" s="241"/>
       <c r="E179" s="289"/>
-      <c r="F179" s="323"/>
+      <c r="F179" s="349"/>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B180" s="325" t="s">
+      <c r="B180" s="338" t="s">
         <v>110</v>
       </c>
       <c r="C180" s="274">
@@ -6802,94 +6805,94 @@
       </c>
       <c r="D180" s="275"/>
       <c r="E180" s="296"/>
-      <c r="F180" s="321">
+      <c r="F180" s="347">
         <f>SUM(E180:E189)</f>
         <v>0</v>
       </c>
     </row>
     <row r="181" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B181" s="326"/>
+      <c r="B181" s="339"/>
       <c r="C181" s="234">
         <v>2</v>
       </c>
       <c r="D181" s="280"/>
       <c r="E181" s="297"/>
-      <c r="F181" s="322"/>
+      <c r="F181" s="348"/>
     </row>
     <row r="182" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B182" s="326"/>
+      <c r="B182" s="339"/>
       <c r="C182" s="234">
         <v>3</v>
       </c>
       <c r="D182" s="280"/>
       <c r="E182" s="297"/>
-      <c r="F182" s="322"/>
+      <c r="F182" s="348"/>
     </row>
     <row r="183" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B183" s="326"/>
+      <c r="B183" s="339"/>
       <c r="C183" s="234">
         <v>4</v>
       </c>
       <c r="D183" s="280"/>
       <c r="E183" s="297"/>
-      <c r="F183" s="322"/>
+      <c r="F183" s="348"/>
     </row>
     <row r="184" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B184" s="326"/>
+      <c r="B184" s="339"/>
       <c r="C184" s="234">
         <v>5</v>
       </c>
       <c r="D184" s="280"/>
       <c r="E184" s="297"/>
-      <c r="F184" s="322"/>
+      <c r="F184" s="348"/>
     </row>
     <row r="185" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B185" s="326"/>
+      <c r="B185" s="339"/>
       <c r="C185" s="234">
         <v>6</v>
       </c>
       <c r="D185" s="280"/>
       <c r="E185" s="297"/>
-      <c r="F185" s="322"/>
+      <c r="F185" s="348"/>
     </row>
     <row r="186" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B186" s="326"/>
+      <c r="B186" s="339"/>
       <c r="C186" s="234">
         <v>7</v>
       </c>
       <c r="D186" s="280"/>
       <c r="E186" s="297"/>
-      <c r="F186" s="322"/>
+      <c r="F186" s="348"/>
     </row>
     <row r="187" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B187" s="326"/>
+      <c r="B187" s="339"/>
       <c r="C187" s="234">
         <v>8</v>
       </c>
       <c r="D187" s="280"/>
       <c r="E187" s="297"/>
-      <c r="F187" s="322"/>
+      <c r="F187" s="348"/>
     </row>
     <row r="188" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B188" s="326"/>
+      <c r="B188" s="339"/>
       <c r="C188" s="234">
         <v>9</v>
       </c>
       <c r="D188" s="280"/>
       <c r="E188" s="297"/>
-      <c r="F188" s="322"/>
+      <c r="F188" s="348"/>
     </row>
     <row r="189" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B189" s="327"/>
+      <c r="B189" s="340"/>
       <c r="C189" s="282">
         <v>10</v>
       </c>
       <c r="D189" s="283"/>
       <c r="E189" s="298"/>
-      <c r="F189" s="323"/>
+      <c r="F189" s="349"/>
     </row>
     <row r="190" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B190" s="325" t="s">
+      <c r="B190" s="338" t="s">
         <v>290</v>
       </c>
       <c r="C190" s="274">
@@ -6897,99 +6900,99 @@
       </c>
       <c r="D190" s="275"/>
       <c r="E190" s="296"/>
-      <c r="F190" s="321">
+      <c r="F190" s="347">
         <f>SUM(E190:E199)</f>
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B191" s="326"/>
+      <c r="B191" s="339"/>
       <c r="C191" s="234">
         <v>2</v>
       </c>
       <c r="D191" s="280"/>
       <c r="E191" s="297"/>
-      <c r="F191" s="322"/>
+      <c r="F191" s="348"/>
     </row>
     <row r="192" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B192" s="326"/>
+      <c r="B192" s="339"/>
       <c r="C192" s="234">
         <v>3</v>
       </c>
       <c r="D192" s="280"/>
       <c r="E192" s="297"/>
-      <c r="F192" s="322"/>
+      <c r="F192" s="348"/>
     </row>
     <row r="193" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B193" s="326"/>
+      <c r="B193" s="339"/>
       <c r="C193" s="234">
         <v>4</v>
       </c>
       <c r="D193" s="280"/>
       <c r="E193" s="297"/>
-      <c r="F193" s="322"/>
+      <c r="F193" s="348"/>
     </row>
     <row r="194" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B194" s="326"/>
+      <c r="B194" s="339"/>
       <c r="C194" s="234">
         <v>5</v>
       </c>
       <c r="D194" s="280"/>
       <c r="E194" s="297"/>
-      <c r="F194" s="322"/>
+      <c r="F194" s="348"/>
     </row>
     <row r="195" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B195" s="326"/>
+      <c r="B195" s="339"/>
       <c r="C195" s="234">
         <v>6</v>
       </c>
       <c r="D195" s="280"/>
       <c r="E195" s="297"/>
-      <c r="F195" s="322"/>
+      <c r="F195" s="348"/>
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B196" s="326"/>
+      <c r="B196" s="339"/>
       <c r="C196" s="234">
         <v>7</v>
       </c>
       <c r="D196" s="280"/>
       <c r="E196" s="297"/>
-      <c r="F196" s="322"/>
+      <c r="F196" s="348"/>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B197" s="326"/>
+      <c r="B197" s="339"/>
       <c r="C197" s="234">
         <v>8</v>
       </c>
       <c r="D197" s="280"/>
       <c r="E197" s="297"/>
-      <c r="F197" s="322"/>
+      <c r="F197" s="348"/>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B198" s="326"/>
+      <c r="B198" s="339"/>
       <c r="C198" s="234">
         <v>9</v>
       </c>
       <c r="D198" s="280"/>
       <c r="E198" s="297"/>
-      <c r="F198" s="322"/>
+      <c r="F198" s="348"/>
     </row>
     <row r="199" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B199" s="327"/>
+      <c r="B199" s="340"/>
       <c r="C199" s="282">
         <v>10</v>
       </c>
       <c r="D199" s="283"/>
       <c r="E199" s="298"/>
-      <c r="F199" s="323"/>
+      <c r="F199" s="349"/>
     </row>
     <row r="200" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B200" s="316" t="s">
+      <c r="B200" s="350" t="s">
         <v>291</v>
       </c>
-      <c r="C200" s="317"/>
-      <c r="D200" s="317"/>
-      <c r="E200" s="318"/>
+      <c r="C200" s="351"/>
+      <c r="D200" s="351"/>
+      <c r="E200" s="352"/>
       <c r="F200" s="299">
         <f>SUM(F99:F199)</f>
         <v>0</v>
@@ -6997,30 +7000,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B10:B16"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B23:B47"/>
-    <mergeCell ref="B99:B108"/>
-    <mergeCell ref="F99:F108"/>
-    <mergeCell ref="B49:B94"/>
-    <mergeCell ref="D49:D94"/>
-    <mergeCell ref="B109:B118"/>
-    <mergeCell ref="F109:F118"/>
-    <mergeCell ref="B119:B128"/>
-    <mergeCell ref="F119:F128"/>
-    <mergeCell ref="B129:B131"/>
-    <mergeCell ref="F129:F131"/>
-    <mergeCell ref="B132:B140"/>
-    <mergeCell ref="F132:F140"/>
-    <mergeCell ref="B141:B150"/>
-    <mergeCell ref="F141:F150"/>
-    <mergeCell ref="B151:B160"/>
-    <mergeCell ref="F151:F160"/>
-    <mergeCell ref="B190:B199"/>
-    <mergeCell ref="F190:F199"/>
     <mergeCell ref="B200:E200"/>
     <mergeCell ref="B161:B170"/>
     <mergeCell ref="F161:F170"/>
@@ -7028,6 +7007,30 @@
     <mergeCell ref="F171:F179"/>
     <mergeCell ref="B180:B189"/>
     <mergeCell ref="F180:F189"/>
+    <mergeCell ref="B141:B150"/>
+    <mergeCell ref="F141:F150"/>
+    <mergeCell ref="B151:B160"/>
+    <mergeCell ref="F151:F160"/>
+    <mergeCell ref="B190:B199"/>
+    <mergeCell ref="F190:F199"/>
+    <mergeCell ref="B119:B128"/>
+    <mergeCell ref="F119:F128"/>
+    <mergeCell ref="B129:B131"/>
+    <mergeCell ref="F129:F131"/>
+    <mergeCell ref="B132:B140"/>
+    <mergeCell ref="F132:F140"/>
+    <mergeCell ref="B99:B108"/>
+    <mergeCell ref="F99:F108"/>
+    <mergeCell ref="B49:B94"/>
+    <mergeCell ref="D49:D94"/>
+    <mergeCell ref="B109:B118"/>
+    <mergeCell ref="F109:F118"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B23:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7055,50 +7058,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="353"/>
-      <c r="B1" s="353"/>
-      <c r="C1" s="353"/>
-      <c r="D1" s="353"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="353"/>
+      <c r="A1" s="362"/>
+      <c r="B1" s="362"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="362"/>
+      <c r="F1" s="362"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="353"/>
-      <c r="B2" s="353"/>
-      <c r="C2" s="353"/>
-      <c r="D2" s="353"/>
-      <c r="E2" s="353"/>
-      <c r="F2" s="353"/>
+      <c r="A2" s="362"/>
+      <c r="B2" s="362"/>
+      <c r="C2" s="362"/>
+      <c r="D2" s="362"/>
+      <c r="E2" s="362"/>
+      <c r="F2" s="362"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="354" t="s">
+      <c r="A3" s="363" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="354"/>
-      <c r="C3" s="354"/>
-      <c r="D3" s="354"/>
-      <c r="E3" s="354"/>
-      <c r="F3" s="354"/>
-      <c r="M3" s="363"/>
-      <c r="N3" s="363"/>
-      <c r="O3" s="363"/>
+      <c r="B3" s="363"/>
+      <c r="C3" s="363"/>
+      <c r="D3" s="363"/>
+      <c r="E3" s="363"/>
+      <c r="F3" s="363"/>
+      <c r="M3" s="361"/>
+      <c r="N3" s="361"/>
+      <c r="O3" s="361"/>
     </row>
     <row r="4" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="1">
-      <c r="A4" s="364" t="s">
+      <c r="A4" s="356" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="364"/>
-      <c r="C4" s="364"/>
-      <c r="D4" s="364"/>
-      <c r="E4" s="364"/>
-      <c r="F4" s="364"/>
+      <c r="B4" s="356"/>
+      <c r="C4" s="356"/>
+      <c r="D4" s="356"/>
+      <c r="E4" s="356"/>
+      <c r="F4" s="356"/>
       <c r="H4" s="126"/>
     </row>
     <row r="5" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="355" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="357" t="s">
+      <c r="A5" s="364" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="358" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="89" t="str">
@@ -7120,8 +7123,8 @@
       <c r="H5"/>
     </row>
     <row r="6" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="356"/>
-      <c r="B6" s="358"/>
+      <c r="A6" s="365"/>
+      <c r="B6" s="359"/>
       <c r="C6" s="138">
         <f>Assumptions.1!I18</f>
         <v>0</v>
@@ -7585,12 +7588,12 @@
     <row r="37" spans="1:14" ht="26" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="360" t="s">
+      <c r="C37" s="353" t="s">
         <v>164</v>
       </c>
-      <c r="D37" s="361"/>
-      <c r="E37" s="361"/>
-      <c r="F37" s="362"/>
+      <c r="D37" s="354"/>
+      <c r="E37" s="354"/>
+      <c r="F37" s="355"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="120"/>
@@ -7599,31 +7602,31 @@
       <c r="F38" s="120"/>
     </row>
     <row r="39" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="353"/>
-      <c r="B39" s="353"/>
-      <c r="C39" s="353"/>
-      <c r="D39" s="353"/>
-      <c r="E39" s="353"/>
-      <c r="F39" s="353"/>
+      <c r="A39" s="362"/>
+      <c r="B39" s="362"/>
+      <c r="C39" s="362"/>
+      <c r="D39" s="362"/>
+      <c r="E39" s="362"/>
+      <c r="F39" s="362"/>
     </row>
     <row r="40" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="353"/>
-      <c r="B40" s="353"/>
-      <c r="C40" s="353"/>
-      <c r="D40" s="353"/>
-      <c r="E40" s="353"/>
-      <c r="F40" s="353"/>
+      <c r="A40" s="362"/>
+      <c r="B40" s="362"/>
+      <c r="C40" s="362"/>
+      <c r="D40" s="362"/>
+      <c r="E40" s="362"/>
+      <c r="F40" s="362"/>
     </row>
     <row r="41" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="359" t="str">
+      <c r="A41" s="360" t="str">
         <f>A3</f>
         <v>STEP 2 : BACK GROUND CALCULATION . NOT TO BE VISIBLE TO CUSTOMER</v>
       </c>
-      <c r="B41" s="359"/>
-      <c r="C41" s="359"/>
-      <c r="D41" s="359"/>
-      <c r="E41" s="359"/>
-      <c r="F41" s="359"/>
+      <c r="B41" s="360"/>
+      <c r="C41" s="360"/>
+      <c r="D41" s="360"/>
+      <c r="E41" s="360"/>
+      <c r="F41" s="360"/>
     </row>
     <row r="42" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A42" s="1"/>
@@ -7635,21 +7638,21 @@
       <c r="N42" s="107"/>
     </row>
     <row r="43" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="1">
-      <c r="A43" s="364" t="s">
+      <c r="A43" s="356" t="s">
         <v>218</v>
       </c>
-      <c r="B43" s="364"/>
-      <c r="C43" s="364"/>
-      <c r="D43" s="364"/>
-      <c r="E43" s="364"/>
-      <c r="F43" s="364"/>
+      <c r="B43" s="356"/>
+      <c r="C43" s="356"/>
+      <c r="D43" s="356"/>
+      <c r="E43" s="356"/>
+      <c r="F43" s="356"/>
       <c r="H43" s="126"/>
     </row>
     <row r="44" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="357" t="s">
+      <c r="A44" s="358" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="357" t="s">
+      <c r="B44" s="358" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="89" t="str">
@@ -7670,8 +7673,8 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="358"/>
-      <c r="B45" s="358"/>
+      <c r="A45" s="359"/>
+      <c r="B45" s="359"/>
       <c r="C45" s="138">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7849,12 +7852,12 @@
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:10" ht="26" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C61" s="360" t="s">
+      <c r="C61" s="353" t="s">
         <v>164</v>
       </c>
-      <c r="D61" s="361"/>
-      <c r="E61" s="361"/>
-      <c r="F61" s="362"/>
+      <c r="D61" s="354"/>
+      <c r="E61" s="354"/>
+      <c r="F61" s="355"/>
     </row>
     <row r="62" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="43" t="s">
@@ -8054,12 +8057,12 @@
       <c r="F76" s="7"/>
     </row>
     <row r="77" spans="1:14" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C77" s="360" t="s">
+      <c r="C77" s="353" t="s">
         <v>164</v>
       </c>
-      <c r="D77" s="361"/>
-      <c r="E77" s="361"/>
-      <c r="F77" s="362"/>
+      <c r="D77" s="354"/>
+      <c r="E77" s="354"/>
+      <c r="F77" s="355"/>
       <c r="I77" s="132"/>
       <c r="J77" s="132"/>
       <c r="K77" s="132"/>
@@ -8068,15 +8071,15 @@
       <c r="N77" s="133"/>
     </row>
     <row r="78" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A78" s="359" t="str">
+      <c r="A78" s="360" t="str">
         <f>A41</f>
         <v>STEP 2 : BACK GROUND CALCULATION . NOT TO BE VISIBLE TO CUSTOMER</v>
       </c>
-      <c r="B78" s="359"/>
-      <c r="C78" s="359"/>
-      <c r="D78" s="359"/>
-      <c r="E78" s="359"/>
-      <c r="F78" s="359"/>
+      <c r="B78" s="360"/>
+      <c r="C78" s="360"/>
+      <c r="D78" s="360"/>
+      <c r="E78" s="360"/>
+      <c r="F78" s="360"/>
       <c r="I78" s="132"/>
       <c r="J78" s="132"/>
       <c r="K78" s="132"/>
@@ -8085,14 +8088,14 @@
       <c r="N78" s="133"/>
     </row>
     <row r="79" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A79" s="365" t="s">
+      <c r="A79" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="B79" s="365"/>
-      <c r="C79" s="365"/>
-      <c r="D79" s="365"/>
-      <c r="E79" s="365"/>
-      <c r="F79" s="365"/>
+      <c r="B79" s="357"/>
+      <c r="C79" s="357"/>
+      <c r="D79" s="357"/>
+      <c r="E79" s="357"/>
+      <c r="F79" s="357"/>
       <c r="H79" s="132"/>
       <c r="I79" s="132"/>
       <c r="J79" s="132"/>
@@ -8280,35 +8283,35 @@
       <c r="F92" s="7"/>
     </row>
     <row r="93" spans="1:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C93" s="360" t="s">
+      <c r="C93" s="353" t="s">
         <v>164</v>
       </c>
-      <c r="D93" s="361"/>
-      <c r="E93" s="361"/>
-      <c r="F93" s="362"/>
+      <c r="D93" s="354"/>
+      <c r="E93" s="354"/>
+      <c r="F93" s="355"/>
       <c r="I93" s="6"/>
     </row>
     <row r="94" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="359" t="str">
+      <c r="A94" s="360" t="str">
         <f>A78</f>
         <v>STEP 2 : BACK GROUND CALCULATION . NOT TO BE VISIBLE TO CUSTOMER</v>
       </c>
-      <c r="B94" s="359"/>
-      <c r="C94" s="359"/>
-      <c r="D94" s="359"/>
-      <c r="E94" s="359"/>
-      <c r="F94" s="359"/>
+      <c r="B94" s="360"/>
+      <c r="C94" s="360"/>
+      <c r="D94" s="360"/>
+      <c r="E94" s="360"/>
+      <c r="F94" s="360"/>
       <c r="I94" s="6"/>
     </row>
     <row r="95" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="365" t="s">
+      <c r="A95" s="357" t="s">
         <v>220</v>
       </c>
-      <c r="B95" s="365"/>
-      <c r="C95" s="365"/>
-      <c r="D95" s="365"/>
-      <c r="E95" s="365"/>
-      <c r="F95" s="365"/>
+      <c r="B95" s="357"/>
+      <c r="C95" s="357"/>
+      <c r="D95" s="357"/>
+      <c r="E95" s="357"/>
+      <c r="F95" s="357"/>
     </row>
     <row r="96" spans="1:12" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A96" s="57"/>
@@ -8414,12 +8417,12 @@
       <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C104" s="360" t="s">
+      <c r="C104" s="353" t="s">
         <v>164</v>
       </c>
-      <c r="D104" s="361"/>
-      <c r="E104" s="361"/>
-      <c r="F104" s="362"/>
+      <c r="D104" s="354"/>
+      <c r="E104" s="354"/>
+      <c r="F104" s="355"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="188" t="s">
@@ -8527,6 +8530,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="C37:F37"/>
     <mergeCell ref="C93:F93"/>
     <mergeCell ref="C104:F104"/>
     <mergeCell ref="A43:F43"/>
@@ -8537,18 +8552,6 @@
     <mergeCell ref="A78:F78"/>
     <mergeCell ref="A94:F94"/>
     <mergeCell ref="C61:F61"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.39370078740157483" bottom="0.3" header="0.23622047244094491" footer="0.16"/>
@@ -8581,27 +8584,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="353"/>
-      <c r="B1" s="353"/>
-      <c r="C1" s="353"/>
-      <c r="D1" s="353"/>
-      <c r="E1" s="353"/>
+      <c r="A1" s="362"/>
+      <c r="B1" s="362"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="362"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="353"/>
-      <c r="B2" s="353"/>
-      <c r="C2" s="353"/>
-      <c r="D2" s="353"/>
-      <c r="E2" s="353"/>
+      <c r="A2" s="362"/>
+      <c r="B2" s="362"/>
+      <c r="C2" s="362"/>
+      <c r="D2" s="362"/>
+      <c r="E2" s="362"/>
     </row>
     <row r="3" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="359" t="s">
+      <c r="A3" s="360" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="359"/>
-      <c r="C3" s="359"/>
-      <c r="D3" s="359"/>
-      <c r="E3" s="359"/>
+      <c r="B3" s="360"/>
+      <c r="C3" s="360"/>
+      <c r="D3" s="360"/>
+      <c r="E3" s="360"/>
       <c r="L3" s="107"/>
       <c r="M3" s="107"/>
       <c r="N3" s="107"/>
@@ -8617,7 +8620,7 @@
       <c r="G4" s="126"/>
     </row>
     <row r="5" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="355" t="s">
+      <c r="A5" s="364" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="89" t="str">
@@ -8639,7 +8642,7 @@
       <c r="G5"/>
     </row>
     <row r="6" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="356"/>
+      <c r="A6" s="365"/>
       <c r="B6" s="138">
         <f>wp!C45</f>
         <v>0</v>
@@ -9826,11 +9829,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="D33:J33"/>
     <mergeCell ref="D34:J34"/>
     <mergeCell ref="D16:J16"/>
     <mergeCell ref="D18:J21"/>
@@ -9840,6 +9838,11 @@
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="D32:J32"/>
     <mergeCell ref="E30:I30"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="D33:J33"/>
   </mergeCells>
   <pageMargins left="0.26" right="0.17" top="0.43307086614173229" bottom="0.2" header="0.31496062992125984" footer="0.16"/>
   <pageSetup scale="87" orientation="portrait" r:id="rId1"/>
@@ -9864,37 +9867,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="353">
+      <c r="A1" s="362">
         <f>Assumptions.1!I3</f>
         <v>0</v>
       </c>
-      <c r="B1" s="353"/>
-      <c r="C1" s="353"/>
-      <c r="D1" s="353"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="353"/>
+      <c r="B1" s="362"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="362"/>
+      <c r="F1" s="362"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="353">
+      <c r="A2" s="362">
         <f>Assumptions.1!I5</f>
         <v>0</v>
       </c>
-      <c r="B2" s="353"/>
-      <c r="C2" s="353"/>
-      <c r="D2" s="353"/>
-      <c r="E2" s="353"/>
-      <c r="F2" s="353"/>
+      <c r="B2" s="362"/>
+      <c r="C2" s="362"/>
+      <c r="D2" s="362"/>
+      <c r="E2" s="362"/>
+      <c r="F2" s="362"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="353">
+      <c r="A3" s="362">
         <f>Assumptions.1!I6</f>
         <v>0</v>
       </c>
-      <c r="B3" s="353"/>
-      <c r="C3" s="353"/>
-      <c r="D3" s="353"/>
-      <c r="E3" s="353"/>
-      <c r="F3" s="353"/>
+      <c r="B3" s="362"/>
+      <c r="C3" s="362"/>
+      <c r="D3" s="362"/>
+      <c r="E3" s="362"/>
+      <c r="F3" s="362"/>
       <c r="M3" s="107"/>
       <c r="N3" s="107"/>
       <c r="O3" s="107"/>
@@ -9911,10 +9914,10 @@
       <c r="H4" s="126"/>
     </row>
     <row r="5" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="355" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="357" t="s">
+      <c r="A5" s="364" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="358" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="89" t="str">
@@ -9936,8 +9939,8 @@
       <c r="H5"/>
     </row>
     <row r="6" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="356"/>
-      <c r="B6" s="358"/>
+      <c r="A6" s="365"/>
+      <c r="B6" s="359"/>
       <c r="C6" s="138">
         <f>FinalWorkings!B6</f>
         <v>0</v>
@@ -10412,37 +10415,37 @@
       <c r="F37" s="120"/>
     </row>
     <row r="38" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="353">
+      <c r="A38" s="362">
         <f>A1</f>
         <v>0</v>
       </c>
-      <c r="B38" s="353"/>
-      <c r="C38" s="353"/>
-      <c r="D38" s="353"/>
-      <c r="E38" s="353"/>
-      <c r="F38" s="353"/>
+      <c r="B38" s="362"/>
+      <c r="C38" s="362"/>
+      <c r="D38" s="362"/>
+      <c r="E38" s="362"/>
+      <c r="F38" s="362"/>
     </row>
     <row r="39" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="353">
+      <c r="A39" s="362">
         <f>A2</f>
         <v>0</v>
       </c>
-      <c r="B39" s="353"/>
-      <c r="C39" s="353"/>
-      <c r="D39" s="353"/>
-      <c r="E39" s="353"/>
-      <c r="F39" s="353"/>
+      <c r="B39" s="362"/>
+      <c r="C39" s="362"/>
+      <c r="D39" s="362"/>
+      <c r="E39" s="362"/>
+      <c r="F39" s="362"/>
     </row>
     <row r="40" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="353">
+      <c r="A40" s="362">
         <f>A3</f>
         <v>0</v>
       </c>
-      <c r="B40" s="353"/>
-      <c r="C40" s="353"/>
-      <c r="D40" s="353"/>
-      <c r="E40" s="353"/>
-      <c r="F40" s="353"/>
+      <c r="B40" s="362"/>
+      <c r="C40" s="362"/>
+      <c r="D40" s="362"/>
+      <c r="E40" s="362"/>
+      <c r="F40" s="362"/>
     </row>
     <row r="41" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A41" s="1"/>
@@ -10465,10 +10468,10 @@
       <c r="H42" s="126"/>
     </row>
     <row r="43" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="357" t="s">
+      <c r="A43" s="358" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="357" t="s">
+      <c r="B43" s="358" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="89" t="str">
@@ -10489,8 +10492,8 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A44" s="358"/>
-      <c r="B44" s="358"/>
+      <c r="A44" s="359"/>
+      <c r="B44" s="359"/>
       <c r="C44" s="138">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -11189,6 +11192,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A38:F38"/>
@@ -11197,12 +11206,6 @@
     <mergeCell ref="A42:F42"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.56000000000000005" right="0.15748031496062992" top="0.39370078740157483" bottom="0.44" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>